<commit_message>
Adds QB RSP analysis
</commit_message>
<xml_diff>
--- a/data/1QB/Predraft_Rookies.xlsx
+++ b/data/1QB/Predraft_Rookies.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/28a1ee50a88aa706/python_work/Dynasty_tools/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/28a1ee50a88aa706/python_work/Dynasty_tools/data/1QB/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="114" documentId="8_{F715F125-FACE-4CDD-A872-54B69401BE6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{508D1FCC-9E68-42A6-B871-0A63773CFAA3}"/>
   <bookViews>
-    <workbookView xWindow="1900" yWindow="1900" windowWidth="16200" windowHeight="28060" xr2:uid="{848F5EBF-908A-44A9-800B-7860AC94F392}"/>
+    <workbookView xWindow="450" yWindow="320" windowWidth="18560" windowHeight="13790" xr2:uid="{848F5EBF-908A-44A9-800B-7860AC94F392}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -771,6 +771,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>